<commit_message>
Work on case and PCB (now completely rectangular)
</commit_message>
<xml_diff>
--- a/business/business.xlsx
+++ b/business/business.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\USBKB\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB25FC5-7154-43A0-970A-9B62D25EF916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C048B-34BC-48F3-A417-9313D9BCA0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="332" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2880" yWindow="5310" windowWidth="21600" windowHeight="11280" tabRatio="332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Stock" sheetId="1" r:id="rId1"/>
+    <sheet name="Part List" sheetId="1" r:id="rId1"/>
     <sheet name="Shipping" sheetId="2" r:id="rId2"/>
     <sheet name="Pricing" sheetId="3" r:id="rId3"/>
     <sheet name="Profit and Loss" sheetId="4" r:id="rId4"/>
-    <sheet name="Business Cost" sheetId="5" r:id="rId5"/>
+    <sheet name="Startup Cost" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
   <si>
     <t>Item</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Case</t>
+  </si>
+  <si>
+    <t>O-Ring</t>
+  </si>
+  <si>
+    <t>https://www.amazon.co.uk/Sumind-Keyboard-Dampeners-Plastic-Mechanical/dp/B0761TSWF3/</t>
   </si>
 </sst>
 </file>
@@ -341,7 +347,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -356,6 +362,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -366,13 +374,48 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -435,42 +478,7 @@
       <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,8 +494,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Product" displayName="Product" ref="A1:I17" totalsRowCount="1">
-  <autoFilter ref="A1:I16" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Product" displayName="Product" ref="A1:I18" totalsRowCount="1">
+  <autoFilter ref="A1:I17" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
     <sortCondition descending="1" ref="F1:F15"/>
   </sortState>
@@ -495,13 +503,13 @@
     <tableColumn id="1" xr3:uid="{FC55CD13-AEA3-4A34-8C30-C21DDC109ED5}" name="Item" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{F78DCBEF-EFE2-4614-96AB-F9F26F0F356B}" name="Item Code"/>
     <tableColumn id="3" xr3:uid="{74C2F96D-B077-41FE-97D3-44F2D50D1991}" name="Bulk Amount"/>
-    <tableColumn id="4" xr3:uid="{BE58D40E-C9F3-4603-8913-8D8EDC5D2F3E}" name="Bulk Price" totalsRowFunction="sum" totalsRowDxfId="8" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{BE58D40E-C9F3-4603-8913-8D8EDC5D2F3E}" name="Bulk Price" totalsRowFunction="sum" totalsRowDxfId="1" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{14050057-8386-40CF-8EFF-AA4B79EC4B45}" name="Amount Required"/>
-    <tableColumn id="5" xr3:uid="{A2756D08-6B39-4087-850F-D368262F3916}" name="Price Per Product" totalsRowFunction="sum" totalsRowDxfId="7" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{A2756D08-6B39-4087-850F-D368262F3916}" name="Price Per Product" totalsRowFunction="sum" totalsRowDxfId="0" dataCellStyle="Currency">
       <calculatedColumnFormula>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{EFA10657-4E6F-4746-946B-C366EB641E89}" name="Shipper #"/>
-    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link" dataDxfId="8"/>
     <tableColumn id="8" xr3:uid="{BB457E6F-2E65-4946-B94F-0519D58C2E65}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -514,13 +522,13 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D814D6E7-02BA-4662-8171-E36B08AEDAFC}" name="Shipper #" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{860B23DE-DFF9-4D8E-9CD3-181A9FD87038}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{E159C8E6-48A1-4634-A833-D80999A48180}" name="Shipping Cost" totalsRowDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{C8C73543-E2B5-4932-83DB-BF0A32753EF8}" name="Discount Threshold" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{E159C8E6-48A1-4634-A833-D80999A48180}" name="Shipping Cost" totalsRowDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{C8C73543-E2B5-4932-83DB-BF0A32753EF8}" name="Discount Threshold" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{6F14FEB9-53F9-4CD8-B03C-98E0D999D5B0}" name="Discount %" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{FFD1D024-2F5D-462B-84E6-5D06AB4D8B3E}" name="Total Items Cost" totalsRowDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{FFD1D024-2F5D-462B-84E6-5D06AB4D8B3E}" name="Total Items Cost" totalsRowDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>SUMIF(Product[Shipper '#],  Shipping[[#This Row],[Shipper '#]], Product[Bulk Price])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0E68DB8-28BC-49A8-86E4-AD3CC8775D3A}" name="Final Shipping Cost" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{B0E68DB8-28BC-49A8-86E4-AD3CC8775D3A}" name="Final Shipping Cost" totalsRowFunction="sum" totalsRowDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(Shipping[[#This Row],[Discount Threshold]] &lt;= Shipping[[#This Row],[Total Items Cost]], Shipping[[#This Row],[Shipping Cost]] *(100% - Shipping[[#This Row],[Discount %]]), Shipping[[#This Row],[Shipping Cost]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -556,7 +564,7 @@
   <autoFilter ref="A1:B5" xr:uid="{7B666BC8-EA6C-4259-AC78-5701EA26F788}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C05490DE-0DBF-4579-8E0A-0B5BEEA8F6F2}" name="Title" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{2EB7FFE6-45DB-434A-89FC-6ADAD146844C}" name="€" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="2" totalsRowCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{2EB7FFE6-45DB-434A-89FC-6ADAD146844C}" name="€" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Product[[#Totals],[Bulk Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -827,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +850,7 @@
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="42.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1243,7 +1251,9 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
       <c r="F16" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
         <v>0</v>
@@ -1256,24 +1266,59 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17">
+        <v>800</v>
+      </c>
+      <c r="D17" s="13">
+        <v>14.94</v>
+      </c>
+      <c r="E17">
+        <v>68</v>
+      </c>
+      <c r="F17" s="3">
+        <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
+        <v>1.2699</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D18" s="12">
         <f>SUBTOTAL(109,Product[Bulk Price])</f>
-        <v>441.05599999999998</v>
-      </c>
-      <c r="F17" s="10">
+        <v>455.99599999999998</v>
+      </c>
+      <c r="F18" s="12">
         <f>SUBTOTAL(109,Product[Price Per Product])</f>
-        <v>40.255821991341982</v>
-      </c>
-    </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="1"/>
+        <v>41.525721991341982</v>
+      </c>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F2:F18">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{44E94B3B-2CEB-48DD-8DB8-BCB5AF22E499}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
     <hyperlink ref="H6" r:id="rId2" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
@@ -1294,6 +1339,23 @@
   <tableParts count="1">
     <tablePart r:id="rId15"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{44E94B3B-2CEB-48DD-8DB8-BCB5AF22E499}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F2:F18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1488,7 +1550,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1576,7 @@
       </c>
       <c r="C2" s="4">
         <f>Product[[#Totals],[Price Per Product]]</f>
-        <v>40.255821991341982</v>
+        <v>41.525721991341982</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1549,7 +1611,7 @@
       </c>
       <c r="C6" s="4">
         <f>C5+C2</f>
-        <v>45.867821991341984</v>
+        <v>47.137721991341984</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1566,7 +1628,7 @@
       </c>
       <c r="C8" s="8">
         <f>C6*(1+B7)</f>
-        <v>68.801732987012969</v>
+        <v>70.706582987012979</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1582,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8AB611-8F8B-4554-B957-01DA67DD5EA3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1668,7 @@
       </c>
       <c r="B2" s="4">
         <f>Pricing!C8*Pricing!B3</f>
-        <v>688.01732987012974</v>
+        <v>707.06582987012985</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1615,7 +1677,7 @@
       </c>
       <c r="B3" s="6">
         <f>-Totals[[#Totals],[€]]</f>
-        <v>-497.17599999999999</v>
+        <v>-512.11599999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1624,7 +1686,7 @@
       </c>
       <c r="B4" s="9">
         <f>B2+B3</f>
-        <v>190.84132987012975</v>
+        <v>194.94982987012986</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1641,7 +1703,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,7 +1726,7 @@
       </c>
       <c r="B2" s="5">
         <f>Product[[#Totals],[Bulk Price]]</f>
-        <v>441.05599999999998</v>
+        <v>455.99599999999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1750,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUBTOTAL(109,Totals[€])</f>
-        <v>497.17599999999999</v>
+        <v>512.11599999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to PCB layout, design, diodes, leds, code, everything
</commit_message>
<xml_diff>
--- a/business/business.xlsx
+++ b/business/business.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\USBKB\business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142C048B-34BC-48F3-A417-9313D9BCA0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37024E1-01C9-454C-91BA-6120B93CDF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2880" yWindow="5310" windowWidth="21600" windowHeight="11280" tabRatio="332" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="2400" windowWidth="24345" windowHeight="11790" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part List" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -75,9 +75,6 @@
     <t>22 ohm resistor</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/1005004281845148.html</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -253,6 +250,36 @@
   </si>
   <si>
     <t>https://www.amazon.co.uk/Sumind-Keyboard-Dampeners-Plastic-Mechanical/dp/B0761TSWF3/</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005002631669558.html</t>
+  </si>
+  <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>SK6812 MINI-E</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003546105399.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005004028236758.html</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>1N4148WX-TP</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ie/en/products/detail/micro-commercial-co/1N4148WX-TP/717197</t>
+  </si>
+  <si>
+    <t>NOTE DIGIKEY ORDERS DO NOT INCLUDE VAT</t>
   </si>
 </sst>
 </file>
@@ -358,12 +385,12 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="4" builtinId="3"/>
@@ -374,48 +401,10 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
     </dxf>
     <dxf>
       <font>
@@ -456,9 +445,6 @@
       <numFmt numFmtId="34" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -480,6 +466,15 @@
     <dxf>
       <alignment horizontal="fill" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="_-[$€-1809]* #,##0.00_-;\-[$€-1809]* #,##0.00_-;_-[$€-1809]* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="hh:mm:ss"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -494,10 +489,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Product" displayName="Product" ref="A1:I18" totalsRowCount="1">
-  <autoFilter ref="A1:I17" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
-    <sortCondition descending="1" ref="F1:F15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}" name="Product" displayName="Product" ref="A1:I20" totalsRowCount="1">
+  <autoFilter ref="A1:I19" xr:uid="{A5B2A507-846B-4C1E-857D-6A1DC9B94F2A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I19">
+    <sortCondition descending="1" ref="F1:F19"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FC55CD13-AEA3-4A34-8C30-C21DDC109ED5}" name="Item" totalsRowLabel="Total"/>
@@ -509,7 +504,7 @@
       <calculatedColumnFormula>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{EFA10657-4E6F-4746-946B-C366EB641E89}" name="Shipper #"/>
-    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{BE90050D-FF28-4B34-9EF1-38D899405D92}" name="Link" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{BB457E6F-2E65-4946-B94F-0519D58C2E65}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -517,18 +512,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}" name="Shipping" displayName="Shipping" ref="A1:G7" totalsRowCount="1">
-  <autoFilter ref="A1:G6" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}" name="Shipping" displayName="Shipping" ref="A1:G8" totalsRowCount="1">
+  <autoFilter ref="A1:G7" xr:uid="{8FE08B54-EF1B-4ED2-A73F-DBC0452C2048}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D814D6E7-02BA-4662-8171-E36B08AEDAFC}" name="Shipper #" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{860B23DE-DFF9-4D8E-9CD3-181A9FD87038}" name="Name"/>
-    <tableColumn id="3" xr3:uid="{E159C8E6-48A1-4634-A833-D80999A48180}" name="Shipping Cost" totalsRowDxfId="7" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{C8C73543-E2B5-4932-83DB-BF0A32753EF8}" name="Discount Threshold" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E159C8E6-48A1-4634-A833-D80999A48180}" name="Shipping Cost" totalsRowDxfId="4" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{C8C73543-E2B5-4932-83DB-BF0A32753EF8}" name="Discount Threshold" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{6F14FEB9-53F9-4CD8-B03C-98E0D999D5B0}" name="Discount %" dataCellStyle="Percent"/>
-    <tableColumn id="7" xr3:uid="{FFD1D024-2F5D-462B-84E6-5D06AB4D8B3E}" name="Total Items Cost" totalsRowDxfId="5" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{FFD1D024-2F5D-462B-84E6-5D06AB4D8B3E}" name="Total Items Cost" totalsRowDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>SUMIF(Product[Shipper '#],  Shipping[[#This Row],[Shipper '#]], Product[Bulk Price])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B0E68DB8-28BC-49A8-86E4-AD3CC8775D3A}" name="Final Shipping Cost" totalsRowFunction="sum" totalsRowDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{B0E68DB8-28BC-49A8-86E4-AD3CC8775D3A}" name="Final Shipping Cost" totalsRowFunction="sum" totalsRowDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(Shipping[[#This Row],[Discount Threshold]] &lt;= Shipping[[#This Row],[Total Items Cost]], Shipping[[#This Row],[Shipping Cost]] *(100% - Shipping[[#This Row],[Discount %]]), Shipping[[#This Row],[Shipping Cost]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -564,7 +559,7 @@
   <autoFilter ref="A1:B5" xr:uid="{7B666BC8-EA6C-4259-AC78-5701EA26F788}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C05490DE-0DBF-4579-8E0A-0B5BEEA8F6F2}" name="Title" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{2EB7FFE6-45DB-434A-89FC-6ADAD146844C}" name="€" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2" totalsRowCellStyle="Comma">
+    <tableColumn id="2" xr3:uid="{2EB7FFE6-45DB-434A-89FC-6ADAD146844C}" name="€" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6" totalsRowCellStyle="Comma">
       <calculatedColumnFormula>Product[[#Totals],[Bulk Price]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -835,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,8 +845,8 @@
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="41" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -868,331 +863,329 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
       </c>
       <c r="H1" t="s">
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C2">
-        <v>770</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3">
-        <v>125.11</v>
+        <v>450</v>
       </c>
       <c r="E2">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="F2" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>11.048675324675324</v>
+        <v>45</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2" s="11" t="s">
-        <v>23</v>
+      <c r="H2" s="10"/>
+      <c r="I2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <v>67.896000000000001</v>
+        <v>156.54</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>6.7896000000000001</v>
+        <v>15.654</v>
       </c>
       <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>53</v>
+        <v>0</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>660</v>
       </c>
       <c r="D4" s="3">
-        <v>54.6</v>
+        <v>114.11</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F4" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>5.46</v>
+        <v>10.546530303030304</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11" t="s">
         <v>6</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C5">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3">
-        <v>75.91</v>
+        <v>67.896000000000001</v>
       </c>
       <c r="E5">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="F5" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>5.16188</v>
+        <v>6.7896000000000001</v>
       </c>
       <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3">
-        <v>2.67</v>
+        <v>54.6</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>2.67</v>
+        <v>5.46</v>
       </c>
       <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="3">
-        <v>25.91</v>
+        <v>75.91</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>2.5910000000000002</v>
+        <v>4.6305100000000001</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3">
-        <v>35.42</v>
+        <v>40.56</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>1.1806666666666668</v>
+        <v>4.056</v>
       </c>
       <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>700</v>
       </c>
       <c r="D9" s="3">
-        <v>6.64</v>
+        <v>40.61</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F9" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>0.66399999999999992</v>
+        <v>3.5388714285714284</v>
       </c>
       <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>10</v>
       </c>
       <c r="D10" s="3">
-        <v>3.67</v>
+        <v>25.91</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>0.36699999999999999</v>
+        <v>2.5910000000000002</v>
       </c>
       <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>610</v>
       </c>
       <c r="D11" s="3">
-        <v>1.34</v>
+        <v>18.350000000000001</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>0.13400000000000001</v>
+        <v>1.8350000000000002</v>
       </c>
       <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D12" s="3">
-        <v>0.99</v>
+        <v>35.42</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>9.9000000000000005E-2</v>
+        <v>1.1806666666666668</v>
       </c>
       <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>31</v>
+        <v>3</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C13">
-        <v>20</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.34</v>
+        <v>720</v>
+      </c>
+      <c r="D13" s="12">
+        <v>13.65</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>3.4000000000000002E-2</v>
+        <v>1.1564583333333334</v>
       </c>
       <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1200,113 +1193,183 @@
         <v>68</v>
       </c>
       <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
+        <v>800</v>
+      </c>
+      <c r="D14" s="12">
+        <v>14.94</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="F14" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
+        <v>1.1391749999999998</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14" s="11"/>
+      <c r="H14" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
       </c>
       <c r="C15">
         <v>10</v>
       </c>
       <c r="D15" s="3">
-        <v>40.56</v>
+        <v>6.64</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>4.056</v>
+        <v>0.66399999999999992</v>
       </c>
       <c r="G15">
-        <v>5</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>66</v>
+        <v>1</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
       </c>
       <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3.67</v>
+      </c>
+      <c r="E16">
         <v>1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0</v>
       </c>
       <c r="F16" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>0</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="11"/>
-      <c r="I16" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
       </c>
       <c r="C17">
-        <v>800</v>
-      </c>
-      <c r="D17" s="13">
-        <v>14.94</v>
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.34</v>
       </c>
       <c r="E17">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3">
         <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
-        <v>1.2699</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>70</v>
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.99</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <f>(Product[[#This Row],[Bulk Price]] * Product[[#This Row],[Amount Required]])/Product[[#This Row],[Bulk Amount]]</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D20" s="11">
         <f>SUBTOTAL(109,Product[Bulk Price])</f>
-        <v>455.99599999999998</v>
-      </c>
-      <c r="F18" s="12">
+        <v>1121.4760000000001</v>
+      </c>
+      <c r="F20" s="11">
         <f>SUBTOTAL(109,Product[Price Per Product])</f>
-        <v>41.525721991341982</v>
-      </c>
-    </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="1"/>
+        <v>104.87581173160171</v>
+      </c>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F18">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="F2:F20">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1320,24 +1383,25 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
-    <hyperlink ref="H6" r:id="rId2" xr:uid="{EC767F74-82FC-4314-BC60-145D2B2C7A73}"/>
-    <hyperlink ref="H8" r:id="rId3" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
-    <hyperlink ref="H10" r:id="rId5" xr:uid="{2FADE902-C41E-4F62-814B-4CBC27CB74BF}"/>
-    <hyperlink ref="H13" r:id="rId6" xr:uid="{EBF092F7-4654-4215-BB30-5ACA4BF98616}"/>
-    <hyperlink ref="H5" r:id="rId7" xr:uid="{824C53BE-A827-4F48-A2E2-FAEA1D9288BF}"/>
-    <hyperlink ref="H2" r:id="rId8" xr:uid="{217CF86B-66F4-4978-B9C5-15E745E2F383}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{DAC57D90-EE96-4138-A68F-87F2DB50DF21}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{3A41249C-F5A4-4F54-85B0-1408C3755E91}"/>
-    <hyperlink ref="H9" r:id="rId11" xr:uid="{9E83D466-86BD-44A5-A4F1-D66641DB8063}"/>
-    <hyperlink ref="H3" r:id="rId12" xr:uid="{819B46EC-457A-4B90-B3C3-1A506CB1FB98}"/>
-    <hyperlink ref="H15" r:id="rId13" xr:uid="{E1EBD639-6BAB-4865-A74C-67C8BC2F4A79}"/>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{87CADB05-70DA-4477-979A-5E1D6F664E29}"/>
+    <hyperlink ref="H12" r:id="rId2" xr:uid="{36975494-8557-4D32-AD82-8E0F81F270C6}"/>
+    <hyperlink ref="H10" r:id="rId3" xr:uid="{72D62951-C1A1-4B07-A242-B0E2D08EF3D6}"/>
+    <hyperlink ref="H16" r:id="rId4" xr:uid="{2FADE902-C41E-4F62-814B-4CBC27CB74BF}"/>
+    <hyperlink ref="H19" r:id="rId5" xr:uid="{EBF092F7-4654-4215-BB30-5ACA4BF98616}"/>
+    <hyperlink ref="H7" r:id="rId6" xr:uid="{824C53BE-A827-4F48-A2E2-FAEA1D9288BF}"/>
+    <hyperlink ref="H4" r:id="rId7" xr:uid="{217CF86B-66F4-4978-B9C5-15E745E2F383}"/>
+    <hyperlink ref="H17" r:id="rId8" xr:uid="{DAC57D90-EE96-4138-A68F-87F2DB50DF21}"/>
+    <hyperlink ref="H18" r:id="rId9" xr:uid="{3A41249C-F5A4-4F54-85B0-1408C3755E91}"/>
+    <hyperlink ref="H15" r:id="rId10" xr:uid="{9E83D466-86BD-44A5-A4F1-D66641DB8063}"/>
+    <hyperlink ref="H5" r:id="rId11" xr:uid="{819B46EC-457A-4B90-B3C3-1A506CB1FB98}"/>
+    <hyperlink ref="H8" r:id="rId12" xr:uid="{E1EBD639-6BAB-4865-A74C-67C8BC2F4A79}"/>
+    <hyperlink ref="H14" r:id="rId13" xr:uid="{B180FCBC-5576-4C9F-87B1-E907760A55A9}"/>
+    <hyperlink ref="H11" r:id="rId14" xr:uid="{469ADBA8-EC6F-4B01-BCD7-0DF72A8EF968}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
   <tableParts count="1">
-    <tablePart r:id="rId15"/>
+    <tablePart r:id="rId16"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -1351,7 +1415,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F2:F18</xm:sqref>
+          <xm:sqref>F2:F20</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1361,10 +1425,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9924E6D-4D6E-4392-B6FD-F79E78323971}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,25 +1444,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1406,7 +1470,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="3">
         <v>18</v>
@@ -1431,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3">
         <v>21</v>
@@ -1456,7 +1520,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="3">
         <v>6.15</v>
@@ -1481,7 +1545,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3">
         <v>23</v>
@@ -1506,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3">
         <v>5.97</v>
@@ -1527,14 +1591,39 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6.92</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUMIF(Product[Shipper '#],  Shipping[[#This Row],[Shipper '#]], Product[Bulk Price])</f>
+        <v>114.11</v>
+      </c>
+      <c r="G7" s="3">
+        <f>IF(Shipping[[#This Row],[Discount Threshold]] &lt;= Shipping[[#This Row],[Total Items Cost]], Shipping[[#This Row],[Shipping Cost]] *(100% - Shipping[[#This Row],[Discount %]]), Shipping[[#This Row],[Shipping Cost]])</f>
+        <v>6.92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10">
+      <c r="C8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13">
         <f>SUBTOTAL(109,Shipping[Final Shipping Cost])</f>
-        <v>56.12</v>
+        <v>63.04</v>
       </c>
     </row>
   </sheetData>
@@ -1550,38 +1639,39 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4">
         <f>Product[[#Totals],[Price Per Product]]</f>
-        <v>41.525721991341982</v>
+        <v>104.87581173160171</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1589,34 +1679,34 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4">
         <f>Shipping[[#Totals],[Final Shipping Cost]]</f>
-        <v>56.12</v>
+        <v>63.04</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="6">
         <f>B4/B3</f>
-        <v>5.6120000000000001</v>
+        <v>6.3040000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="4">
         <f>C5+C2</f>
-        <v>47.137721991341984</v>
+        <v>111.17981173160172</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="7">
         <v>0.5</v>
@@ -1624,11 +1714,11 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="8">
         <f>C6*(1+B7)</f>
-        <v>70.706582987012979</v>
+        <v>166.76971759740258</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1645,48 +1735,48 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="4">
         <f>Pricing!C8*Pricing!B3</f>
-        <v>707.06582987012985</v>
+        <v>1667.6971759740259</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6">
         <f>-Totals[[#Totals],[€]]</f>
-        <v>-512.11599999999999</v>
+        <v>-1184.5160000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="9">
         <f>B2+B3</f>
-        <v>194.94982987012986</v>
+        <v>483.18117597402579</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1703,39 +1793,39 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="5">
         <f>Product[[#Totals],[Bulk Price]]</f>
-        <v>455.99599999999998</v>
+        <v>1121.4760000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="5">
         <f>Shipping[[#Totals],[Final Shipping Cost]]</f>
-        <v>56.12</v>
+        <v>63.04</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1750,7 +1840,7 @@
       </c>
       <c r="B6" s="5">
         <f>SUBTOTAL(109,Totals[€])</f>
-        <v>512.11599999999999</v>
+        <v>1184.5160000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>